<commit_message>
Added prototyp and fixed library
</commit_message>
<xml_diff>
--- a/Prototyp2/Parts.xlsx
+++ b/Prototyp2/Parts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msa2-my.sharepoint.com/personal/22117_edu_msa_nl/Documents/School/Informatica/LED-Matrix-Display/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msa2-my.sharepoint.com/personal/22117_edu_msa_nl/Documents/School/Informatica/LED-Matrix-Display/Prototyp2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{19C1D236-7B39-48E9-83E0-DE571980523C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DBDEFE1C-07B2-4C5E-A550-7382D094D28E}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{19C1D236-7B39-48E9-83E0-DE571980523C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0BD0AEDF-DAB9-49A8-8E88-B676A76DFA94}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A3:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H10" activeCellId="1" sqref="H5 H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>